<commit_message>
Commit de atualização e correção 24/10/23
</commit_message>
<xml_diff>
--- a/Arquivos/dadosResposta.xlsx
+++ b/Arquivos/dadosResposta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Petronio\Dropbox\Estatística\Meus Livros\Bioestatística_R\Arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petro\Dropbox\Estatistica\Meus_Livros\bookR\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{748C6056-D89E-4ADA-88F1-17C2C99CEA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467AA3C9-48DC-4F33-A9EE-66D25142BE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11850" yWindow="465" windowWidth="14610" windowHeight="14100" xr2:uid="{894CD224-0E8A-4C68-90B7-FA2BAD270C49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{894CD224-0E8A-4C68-90B7-FA2BAD270C49}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,32 +512,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>0.98</v>
+        <v>1.63</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1.1100000000000001</v>
+        <v>1.97</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1.27</v>
+        <v>0.98</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>1.32</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>1.44</v>
+        <v>1.27</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -567,10 +567,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>1.45</v>
+        <v>1.32</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -578,10 +578,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>1.46</v>
+        <v>1.44</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -589,54 +589,54 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>1.63</v>
+        <v>1.45</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>1.69</v>
+        <v>1.46</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>1.71</v>
+        <v>1.76</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>1.75</v>
+        <v>2.56</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>1.76</v>
+        <v>3.07</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -644,10 +644,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>1.83</v>
+        <v>1.69</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -655,21 +655,21 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>1.97</v>
+        <v>1.71</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>1.97</v>
+        <v>1.75</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -677,10 +677,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>2.5299999999999998</v>
+        <v>1.83</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -688,21 +688,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>2.56</v>
+        <v>1.97</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>2.66</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -710,10 +710,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>2.91</v>
+        <v>2.66</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -721,18 +721,18 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>3.07</v>
+        <v>2.91</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>3.28</v>
@@ -753,6 +753,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>